<commit_message>
ABM Varios (Clientes, etc)
Se dieron de alta varios ABMs
</commit_message>
<xml_diff>
--- a/documentacion/Documentos/Mejoras 1.0.xlsx
+++ b/documentacion/Documentos/Mejoras 1.0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos Colombero\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\mcelitemachines\documentacion\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F742F6-E557-45B8-90BB-A03B174ECEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="articulos" sheetId="3" r:id="rId3"/>
     <sheet name="detalle Produccion" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="159">
   <si>
     <t>Control de stock de materiales</t>
   </si>
@@ -502,13 +501,16 @@
   </si>
   <si>
     <t>Blanco</t>
+  </si>
+  <si>
+    <t>Tiempo Fabricacion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,8 +534,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -567,6 +576,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -642,20 +663,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,7 +994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -990,13 +1015,13 @@
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1226,7 +1251,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -1622,11 +1647,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,114 +1661,117 @@
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="11" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="8">
         <v>777777777</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="8">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="I2" s="10"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1751,19 +1779,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="19"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.7109375" customWidth="1"/>
@@ -1773,976 +1802,976 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="H1" s="12" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="H1" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="9" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="16">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="8">
         <v>6</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10" t="s">
+      <c r="L3" s="8"/>
+      <c r="M3" s="8" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="16">
         <v>16</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="18"/>
+      <c r="F4" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10" t="s">
+      <c r="H4" s="8"/>
+      <c r="I4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="8">
         <v>0.75</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10" t="s">
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="16">
         <v>5</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10" t="s">
+      <c r="E5" s="18"/>
+      <c r="F5" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="8">
         <v>0.2</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10" t="s">
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="16">
         <v>0.5</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="18"/>
+      <c r="F6" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="8">
         <v>0.5</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10" t="s">
+      <c r="L6" s="8"/>
+      <c r="M6" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="16">
         <v>0.2</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="18"/>
+      <c r="F7" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10" t="s">
+      <c r="H7" s="8"/>
+      <c r="I7" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="8">
         <v>0.3</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10" t="s">
+      <c r="L7" s="8"/>
+      <c r="M7" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="16">
         <v>0.5</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="18"/>
+      <c r="F8" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10" t="s">
+      <c r="H8" s="8"/>
+      <c r="I8" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="13" t="s">
+      <c r="J8" s="8"/>
+      <c r="K8" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="16">
         <v>0.5</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="18"/>
+      <c r="F9" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
+      <c r="H9" s="8"/>
+      <c r="I9" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="8">
         <v>0.1</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10" t="s">
+      <c r="L9" s="8"/>
+      <c r="M9" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="16">
         <v>1.7</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10" t="s">
+      <c r="H10" s="8"/>
+      <c r="I10" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="8">
         <v>0.1</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10" t="s">
+      <c r="L10" s="8"/>
+      <c r="M10" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="16">
         <v>1</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10" t="s">
+      <c r="E11" s="18"/>
+      <c r="F11" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="13" t="s">
+      <c r="J11" s="8"/>
+      <c r="K11" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="16">
         <v>0.3</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10" t="s">
+      <c r="E12" s="18"/>
+      <c r="F12" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="8">
         <v>0.1</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10" t="s">
+      <c r="L12" s="8"/>
+      <c r="M12" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="13" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10" t="s">
+      <c r="E13" s="18"/>
+      <c r="F13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="8">
         <v>0.1</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10" t="s">
+      <c r="L13" s="8"/>
+      <c r="M13" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="16">
         <v>0.1</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10" t="s">
+      <c r="E14" s="18"/>
+      <c r="F14" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="8">
         <v>0.1</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10" t="s">
+      <c r="L14" s="8"/>
+      <c r="M14" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="16">
         <v>0.1</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10" t="s">
+      <c r="E15" s="18"/>
+      <c r="F15" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="8">
         <v>0.1</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K15" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10" t="s">
+      <c r="L15" s="8"/>
+      <c r="M15" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="13" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10" t="s">
+      <c r="E16" s="18"/>
+      <c r="F16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="8">
         <v>0.1</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10" t="s">
+      <c r="L16" s="8"/>
+      <c r="M16" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="16">
         <v>0.1</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10" t="s">
+      <c r="E17" s="18"/>
+      <c r="F17" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="8">
         <v>0.5</v>
       </c>
-      <c r="K17" s="13" t="s">
+      <c r="K17" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10" t="s">
+      <c r="L17" s="8"/>
+      <c r="M17" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="16">
         <v>0.1</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10" t="s">
+      <c r="E18" s="18"/>
+      <c r="F18" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="8">
         <v>0.15</v>
       </c>
-      <c r="K18" s="13" t="s">
+      <c r="K18" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10" t="s">
+      <c r="L18" s="8"/>
+      <c r="M18" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="16">
         <v>0.1</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10" t="s">
+      <c r="E19" s="18"/>
+      <c r="F19" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="8">
         <v>0.2</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10" t="s">
+      <c r="L19" s="8"/>
+      <c r="M19" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="16">
         <v>0.1</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10" t="s">
+      <c r="E20" s="18"/>
+      <c r="F20" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="8">
         <v>1</v>
       </c>
-      <c r="K20" s="13" t="s">
+      <c r="K20" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10" t="s">
+      <c r="L20" s="8"/>
+      <c r="M20" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="16">
         <v>0.1</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10" t="s">
+      <c r="E21" s="18"/>
+      <c r="F21" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="8">
         <v>0.1</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K21" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10" t="s">
+      <c r="L21" s="8"/>
+      <c r="M21" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="16">
         <v>1</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10" t="s">
+      <c r="E22" s="18"/>
+      <c r="F22" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="8">
         <v>0.3</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10" t="s">
+      <c r="L22" s="8"/>
+      <c r="M22" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="16">
         <v>0.3</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10" t="s">
+      <c r="E23" s="18"/>
+      <c r="F23" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10" t="s">
+      <c r="H23" s="8"/>
+      <c r="I23" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="8">
         <v>0.3</v>
       </c>
-      <c r="K23" s="13" t="s">
+      <c r="K23" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10" t="s">
+      <c r="L23" s="8"/>
+      <c r="M23" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="16">
         <v>0.2</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10" t="s">
+      <c r="E24" s="18"/>
+      <c r="F24" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10" t="s">
+      <c r="H24" s="8"/>
+      <c r="I24" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="8">
         <v>0.4</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10" t="s">
+      <c r="L24" s="8"/>
+      <c r="M24" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10" t="s">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="16">
         <v>1</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10" t="s">
+      <c r="E25" s="18"/>
+      <c r="F25" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10" t="s">
+      <c r="H25" s="8"/>
+      <c r="I25" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="8">
         <v>4</v>
       </c>
-      <c r="K25" s="13" t="s">
+      <c r="K25" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10" t="s">
+      <c r="L25" s="8"/>
+      <c r="M25" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10" t="s">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="16">
         <v>0.1</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10" t="s">
+      <c r="E26" s="18"/>
+      <c r="F26" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10" t="s">
+      <c r="H26" s="8"/>
+      <c r="I26" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="8">
         <v>0.05</v>
       </c>
-      <c r="K26" s="13" t="s">
+      <c r="K26" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10" t="s">
+      <c r="L26" s="8"/>
+      <c r="M26" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="16">
         <v>0.35</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10" t="s">
+      <c r="E27" s="18"/>
+      <c r="F27" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10" t="s">
+      <c r="H27" s="8"/>
+      <c r="I27" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="J27" s="10">
+      <c r="J27" s="8">
         <v>0.3</v>
       </c>
-      <c r="K27" s="13" t="s">
+      <c r="K27" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10" t="s">
+      <c r="L27" s="8"/>
+      <c r="M27" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10" t="s">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="16">
         <v>0.35</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10" t="s">
+      <c r="E28" s="18"/>
+      <c r="F28" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10" t="s">
+      <c r="H28" s="8"/>
+      <c r="I28" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="13" t="s">
+      <c r="J28" s="8"/>
+      <c r="K28" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10" t="s">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="16">
         <v>0.5</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10" t="s">
+      <c r="E29" s="18"/>
+      <c r="F29" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10" t="s">
+      <c r="H29" s="8"/>
+      <c r="I29" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J29" s="8">
         <v>2</v>
       </c>
-      <c r="K29" s="13" t="s">
+      <c r="K29" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10" t="s">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="16">
         <v>12</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10" t="s">
+      <c r="E30" s="18"/>
+      <c r="F30" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="J30" s="10">
+      <c r="J30" s="8">
         <v>4</v>
       </c>
-      <c r="K30" s="13" t="s">
+      <c r="K30" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10" t="s">
+      <c r="L30" s="8"/>
+      <c r="M30" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10" t="s">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="16">
         <v>0.05</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10" t="s">
+      <c r="E31" s="18"/>
+      <c r="F31" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="J31" s="10">
+      <c r="J31" s="8">
         <v>4</v>
       </c>
-      <c r="K31" s="13" t="s">
+      <c r="K31" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10" t="s">
+      <c r="L31" s="8"/>
+      <c r="M31" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10" t="s">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="16">
         <v>0.35</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10" t="s">
+      <c r="E32" s="18"/>
+      <c r="F32" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10" t="s">
+      <c r="H32" s="8"/>
+      <c r="I32" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="J32" s="10">
+      <c r="J32" s="8">
         <v>0.25</v>
       </c>
-      <c r="K32" s="13" t="s">
+      <c r="K32" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10" t="s">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="13" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10" t="s">
+      <c r="E33" s="18"/>
+      <c r="F33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="J33" s="10">
+      <c r="J33" s="8">
         <v>0.5</v>
       </c>
-      <c r="K33" s="13" t="s">
+      <c r="K33" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10" t="s">
+      <c r="L33" s="8"/>
+      <c r="M33" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10" t="s">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="16">
         <v>2</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10" t="s">
+      <c r="E34" s="18"/>
+      <c r="F34" s="8" t="s">
         <v>110</v>
       </c>
       <c r="M34" t="s">
@@ -2750,174 +2779,174 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="16">
         <v>4</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10" t="s">
+      <c r="E35" s="18"/>
+      <c r="F35" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10" t="s">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="16">
         <v>2</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10" t="s">
+      <c r="E36" s="18"/>
+      <c r="F36" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10" t="s">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="16">
         <v>2</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10" t="s">
+      <c r="E37" s="18"/>
+      <c r="F37" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10" t="s">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="16">
         <v>4</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10" t="s">
+      <c r="E38" s="18"/>
+      <c r="F38" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10" t="s">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="16">
         <v>4</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10" t="s">
+      <c r="E39" s="18"/>
+      <c r="F39" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10" t="s">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="16">
         <v>16</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10" t="s">
+      <c r="E40" s="18"/>
+      <c r="F40" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10" t="s">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="13" t="s">
+      <c r="C41" s="16"/>
+      <c r="D41" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10" t="s">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="16">
         <v>1</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10" t="s">
+      <c r="E42" s="18"/>
+      <c r="F42" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10" t="s">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="16">
         <v>4</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10" t="s">
+      <c r="E43" s="18"/>
+      <c r="F43" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10" t="s">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="16">
         <v>0.25</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10" t="s">
+      <c r="E44" s="18"/>
+      <c r="F44" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10" t="s">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="16">
         <v>0.5</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10" t="s">
+      <c r="E45" s="18"/>
+      <c r="F45" s="8" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2927,5 +2956,6 @@
     <mergeCell ref="H1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>